<commit_message>
DDT with POM without deprecated C#methods
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -868,16 +868,16 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -891,10 +891,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -908,10 +908,10 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>